<commit_message>
"Refactored code to generate and upload planilha, updated styles and templates, and added concurrent futures for parallel processing"
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,9 +458,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="48" customWidth="1" min="1" max="1"/>
-    <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="126" customWidth="1" min="3" max="3"/>
+    <col width="1260" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,340 +483,51 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>HIS Logistic</t>
+          <t>VALE GRANDE INDUSTRIA E COMERCIO DE ALIMENTOS S/A EM RECUPERACAO JUDICIAL DM2 COMERCIAL DE ALIMENTOS LTDA KIMBERLY -CLARK BRASIL INDUSTRIA E COMERCIO DE PRODUTOS DE HIGIENE LTDA PETROM PETROQUIMICA MOGI DAS CRUZES S/A AGCO DO BRASIL SOLUCOES AGRICOLAS LTDA. HOGANAS BRASIL LTDA NITERRA DO BRASIL LTDA. SUSTENTA ALIMENTOS LTDA FABRICA AURICCHIO INDUSTRIA E COMERCIO DE METAIS LTDA NORAL - NORDESTE ALUMINIO LTDA ORANGE SHIPPING AGENCIAMENTO DE CARGA LTDA EMPORIO DO MARMORE IMPORTACAO E EXPORTACAO LTDA M D GLOBAL LOGISTICA INTERNACIONAL LTDA MG2 MARMORES E GRANITOS LTDA RESINAS BOM SUCESSO INDUSTRIA E COMERCIO LTDA AGROARACA INDUSTRIA DE ALIMENTOS LTDA - EM RECUPERACAO JUDICIAL CARRER ALIMENTOS LTDA EM RECUPERACAO JUDICIAL COOPERATIVA DOS CITRICULTORES ECOLOGICOS DO VALE DO CAI LTDA CS3 MARMORES E GRANITOS LTDA MADEIREIRA RIO CLARO LTDA MAGBAN MARMORES E GRANITOS AQUIDABAN LTDA MEGA SHIPPING CARGO SERVICOS LOGISTICOS LTDA MINERACAO COTO COMERCIO IMPORTACAO E EXPORTACAO LTDA PEMAGRAN PEDRAS MARMORES E GRANITOS LTDA PG QUIMICA LTDA RICLAN S.A. THOR NORTE GRANITOS LTDA ABATEDOURO DE BOVINOS SAMPAIO LTDA AGRO EXPORT SEMENTES PAPINI LTDA AGROSUL AGROAVICOLA INDUSTRIAL S.A. ALFA GESTAO DE NEGOCIOS LTDA ANGRAMAR GRANITOS E MARMORES LTDA BENPE COMERCIO</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>(11) 2779-0818</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>SP-102, 70 - Taiaçupeba, Mogi das Cruzes - SP, 08765-340, Brazil</t>
+          <t>Endereço não encontrado</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Amazon Brazil - GRU10</t>
+          <t xml:space="preserve"> IMPORTACAO E EXPORTACAO LTDA. BOA VISTA - ALIMENTOS LTDA EM RECUPERACAO JUDICIAL CACAU FOODS DO BRASIL INDUSTRIA DE ALIMENTOS LTDA CASA GRANDE MINERACAO LTDA CBRAIN INTERNATIONAL AGENCIAMENTO DE CARGAS LTDA CERAMICA SERRA AZUL LTDA CIA. IGUACU DE CAFE SOLUVEL COAMO AGROINDUSTRIAL COOPERATIVA COMIL COTAXE MINERACAO LTDA CROSS TRADING LOGISTICA</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>0800 038 0541</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Av. Pres. Juscelino Kubitschek, 2041 - Vila Olímpia, São Paulo - SP, 04543-011, Brazil</t>
+          <t>Endereço não encontrado</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Google Brasil</t>
+          <t xml:space="preserve"> IMPORTACAO E EXPORTACAO LTDA. ELGIN HDB REFRIGERACAO LTDA ENERGY COMERCIO INTERNACIONAL LTDA FRIGORIFICO INDUSTRIAL VALE DO PIRANGA S/A GRAMAZINI GRANITOS E MARMORES THOMAZINI LTDA HEMOPROT INDUSTRIA E COMERCIO DE PRODUTOS FRIGORIFICOS LTDA IBRAQUIM TECNOLOGIA LTDA INDUSTRIA DE SUCOS SUMO INDUSTRIAL LTDA EM RECUPERACAO JUDICIAL LABAREDA DO CAITITU - COMERCIO DE CAFE LTDA</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>(11) 2395-8400</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Av. Brig. Faria Lima, 3477 - 18º Andar - Itaim Bibi, São Paulo - SP, 04538-133, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>Microsoft Brazil</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>(11) 5504-2155</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Avenida Presidente Juscelino Kubitscheck, 1909 Torre Sul, 16° andar - Vila Nova Conceição, São Paulo - SP, 04543-907, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Apple Computer Brasil</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>(11) 5503-0000</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>R. Leopoldo Couto Magalhães Júnior, 700 - Itaim Bibi, São Paulo - SP, 01454-901, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Samsung Electronics Amazon</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>(19) 4501-2000</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>R. Thomas Nilsen Júnior, 150 - Parque Imperador, Campinas - SP, 13097-105, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Coca-Cola Femsa</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>(11) 93048-9991</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Av. Francisco Ferreira Lopes, 4303 - Vila Jundiai, Mogi das Cruzes - SP, 08745-000, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>Nestlé</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>(11) 5508-4400</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>Av. das Nações Unidas, 17007 - Várzea de Baixo, São Paulo - SP, 04730-090, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Banco Bradesco - Agência 0231</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>(11) 3003-7538</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>Av. Francisco Ferreira Lopes, 2737 - Vila Brás Cubas, Mogi das Cruzes - SP, 08745-000, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>Banco Itaú - Agência 0142</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>3003-0142</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>Av. Voluntário Fernando Pinheiro Franco, 472 - Centro, Mogi das Cruzes - SP, 08710-550, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Mini Mercado Livre</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Não encontrado</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>R. Des. Aderito Pereira da Silva, 142 - Cidade Kemel, São Paulo - SP, 08130-370, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Magazine Luiza</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>(11) 92015-0420</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>R. Dr. Deodato Wertheimer, 1361 - Centro, Mogi das Cruzes - SP, 08710-430, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Banco Santander - Agência 0087 Mogi Das Cruzes</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>0800 702 3535</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Av. Voluntário Fernando Pinheiro Franco, 175 - Centro, Mogi das Cruzes - SP, 08710-500, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>B2W Digital e Direct</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>(11) 95776-2521</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>Rod. Pres. Castello Branco, 106 - Jardim Maria Cristina, Itapevi - SP, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Volkswagen do Brasil</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>0800 019 5775</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>Rod. Anchieta, km 23,5 - Demarchi, São Bernardo do Campo - SP, 09823-901, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>Ford Brasil</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>0800 703 3673</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>Av. Dr. Cardoso de Melo, 1336 - Vila Olímpia, São Paulo - SP, 04548-004, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Fiat Chrysler do Brasil</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>0800 707 1000</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>R. Gasming, 208-432 - Distrito Industrial Paulo Camilo Sul, 32699, Betim - MG, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>M SUPER COMB E LUBRIF LTDA</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>(11) 4794-4400</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>Av. Lourenço de Souza Franco, 959 - Jundiapeba, Mogi das Cruzes - SP, 08750-560, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Vale S/A</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>Não encontrado</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>Rod. Pres. Juscelino Kubitschek, 0 - Vila Verde, Nova Lima - MG, 34000-000, Brazil</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>Embraer</t>
-        </is>
-      </c>
-      <c r="B21" s="3" t="inlineStr">
-        <is>
-          <t>(12) 3927-1000</t>
-        </is>
-      </c>
-      <c r="C21" s="3" t="inlineStr">
-        <is>
-          <t>Av. Brg. Faria Lima, 2170 - Putim, São José dos Campos - SP, 12227-901, Brazil</t>
+          <t>Endereço não encontrado</t>
         </is>
       </c>
     </row>

</xml_diff>